<commit_message>
1 story + priority update
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12225" windowHeight="3855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -27,21 +27,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PBI00x</t>
-  </si>
-  <si>
-    <t>As a … 
-I want to …
-Because …</t>
-  </si>
-  <si>
     <t>Stroy Points</t>
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>1000 - 0</t>
   </si>
   <si>
     <t>Status</t>
@@ -68,9 +57,6 @@
     <t>As an administrator
 I want to make sure not everyone can access the site 
 Because we want to control the user count</t>
-  </si>
-  <si>
-    <t>THE CELL BELOW IS AN EMPTY USER STORY USE IT TO CREATE NEW ONES BUT DO NOT REMOVE IT</t>
   </si>
   <si>
     <t>PBI002</t>
@@ -156,22 +142,12 @@
 Because I want quick</t>
   </si>
   <si>
-    <t>As a user
-I don't want labels to be fixed
-Because I might think of topics of my own</t>
-  </si>
-  <si>
     <t>As an administrator
 I want every saved exercise and its questions to have labels of question-type and topic
 Because the user wants auto-generated tests</t>
   </si>
   <si>
     <t>As a user
-I don't want to add labels to questions (require topic? Auto-copy from exercise?)
-Because I want fast</t>
-  </si>
-  <si>
-    <t>As a user
 When auto-generating a test, I want to narrow potential questions by selecting a category, and then choose what labels to include and exclude, e.g. by (de)selecting related labels in a word cloud
 Because I don't want irrelevant questions</t>
   </si>
@@ -226,6 +202,31 @@
   </si>
   <si>
     <t>PBI020</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>As a user
+I don't want to add a label to every question (require topic? Auto-copy from exercise?)
+Because I want fast</t>
+  </si>
+  <si>
+    <t>As a user
+I don't want labels to be fixed
+Because I might think of topics of my own
+(distinguish between category and (optional) label?)</t>
+  </si>
+  <si>
+    <t>PBI021</t>
+  </si>
+  <si>
+    <t>As a user (history teacher/student)
+I want to make timelines, the events of which are saved and labeled ('war', 'birth', 'France', 'independence', …) for database purposes; I also want to generate timelines from chosen labels which are then customisable; I also want to generate gap-filling exercises from my timelines
+Because teachers want easy customisable timelines, and students want to easily learn timelines</t>
   </si>
 </sst>
 </file>
@@ -249,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,12 +260,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,441 +276,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="45">
     <dxf>
       <fill>
         <patternFill>
@@ -1336,22 +909,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1359,266 +932,322 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4">
+        <v>990</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4">
+        <v>910</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>900</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4">
+        <v>900</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4">
+        <v>900</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="4">
+        <v>900</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4">
+        <v>900</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4">
+        <v>860</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4">
+        <v>850</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4">
+        <v>850</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C13" s="4">
+        <v>720</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4">
+        <v>700</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C15" s="4">
+        <v>700</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C16" s="4">
+        <v>700</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="C17" s="4">
+        <v>650</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C18" s="4">
+        <v>650</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="4">
+        <v>600</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="C20" s="4">
+        <v>510</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4">
+        <v>500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>8</v>
+      <c r="C22" s="4">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1">
-    <sortState ref="A2:E6">
-      <sortCondition ref="A1"/>
+  <autoFilter ref="A1:F28">
+    <sortState ref="A2:F28">
+      <sortCondition descending="1" ref="C1:C28"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2134,27 +1763,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed 'track' to 'follow' + 'progress' to 'results'
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12225" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16890" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -95,11 +95,6 @@
   </si>
   <si>
     <t>As a user
-I want to track my progress by logging in
-Because it's educational</t>
-  </si>
-  <si>
-    <t>As a user
 I want to make tests and share them via a link without logging in
 Because I want quick and simple</t>
   </si>
@@ -107,11 +102,6 @@
     <t>As a user
 I want to take pre-made tests without logging in if I don't need to save my own results
 Because I want quick and simple</t>
-  </si>
-  <si>
-    <t>As a user
-I want to track other users' progress
-Because I want to help others</t>
   </si>
   <si>
     <t>As a new user
@@ -157,11 +147,6 @@
 Because I want to make the life of my users easier</t>
   </si>
   <si>
-    <t>As a user
-I want to inform my teacher (tracker) and the app if a question is irrelevant (and specify why with labels) and exclude it from result calculations (whether this can be done depends on owner of test)
-Because I don't want irrelevant questions and inaccurate results</t>
-  </si>
-  <si>
     <t>PBI007</t>
   </si>
   <si>
@@ -259,6 +244,21 @@
     <t>As a developer
 I want to make and save a simple test
 Because that seems like a good next step</t>
+  </si>
+  <si>
+    <t>As a user
+I want to see prior results by logging in
+Because it's educational</t>
+  </si>
+  <si>
+    <t>As a user
+I want to inform my teacher (owner of test and/or follower) and the app if a question is irrelevant (and specify why with labels) and exclude it from result calculations (whether this can be done depends on owner of test)
+Because I don't want irrelevant questions and inaccurate results</t>
+  </si>
+  <si>
+    <t>As a user
+I want to follow other users' progress (results)
+Because I want to help others</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1009,10 +1009,10 @@
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4">
         <v>998</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="4">
         <v>997</v>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4">
         <v>996</v>
@@ -1051,10 +1051,10 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="4">
         <v>995</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4">
         <v>910</v>
@@ -1093,10 +1093,10 @@
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4">
         <v>900</v>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="4">
         <v>900</v>
@@ -1119,12 +1119,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="4">
         <v>900</v>
@@ -1133,12 +1133,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4">
         <v>900</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4">
         <v>860</v>
@@ -1161,9 +1161,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
@@ -1175,12 +1175,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4">
         <v>720</v>
@@ -1189,12 +1189,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4">
         <v>700</v>
@@ -1203,12 +1203,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4">
         <v>700</v>
@@ -1219,10 +1219,10 @@
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4">
         <v>700</v>
@@ -1231,12 +1231,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4">
         <v>650</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4">
         <v>650</v>
@@ -1259,12 +1259,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C22" s="4">
         <v>600</v>
@@ -1278,7 +1278,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4">
         <v>510</v>
@@ -1301,12 +1301,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" s="4">
         <v>100</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4">
         <v>0</v>
@@ -1329,7 +1329,7 @@
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stripped down features + added temp header
Some features are commented out for now. Added temp header to experiment
with css.
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16890" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16890" windowHeight="3945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,11 +15,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -259,6 +260,14 @@
     <t>As a user
 I want to follow other users' progress (results)
 Because I want to help others</t>
+  </si>
+  <si>
+    <t>PBI026</t>
+  </si>
+  <si>
+    <t>As a user
+I want learning paths that can be made, shared and taken
+Because it maps my progress and/or the progress of my students</t>
   </si>
 </sst>
 </file>
@@ -941,11 +950,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,13 +1284,13 @@
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C23" s="4">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -1289,13 +1298,13 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4">
-        <v>500</v>
+        <v>410</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -1303,13 +1312,13 @@
     </row>
     <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -1317,24 +1326,38 @@
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C27" s="4">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>9</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F28">
-    <sortState ref="A2:F28">
+    <sortState ref="A2:F27">
       <sortCondition descending="1" ref="C1:C28"/>
     </sortState>
   </autoFilter>

</xml_diff>